<commit_message>
sync ET8 up to date 2023-07-14
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartProcessConfig@s.xlsx
+++ b/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartProcessConfig@s.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Id</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>#</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1024,7 @@
   <dimension ref="A3:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.35" outlineLevelCol="3"/>
@@ -1086,10 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" spans="2:4">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="9" s="1" customFormat="1" spans="3:4">
       <c r="C9" s="5">
         <v>4</v>
       </c>
@@ -1097,10 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" spans="2:4">
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="10" s="1" customFormat="1" spans="3:4">
       <c r="C10" s="5">
         <v>5</v>
       </c>
@@ -1108,10 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="2:4">
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="11" s="1" customFormat="1" spans="3:4">
       <c r="C11" s="5">
         <v>6</v>
       </c>
@@ -1119,10 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="2:4">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="12" s="1" customFormat="1" spans="3:4">
       <c r="C12" s="5">
         <v>7</v>
       </c>
@@ -1132,287 +1117,139 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="2:4">
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="5">
-        <v>12</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="3:4">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" s="2" customFormat="1" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5">
-        <v>13</v>
-      </c>
-      <c r="D18" s="5">
-        <v>1</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:4">
       <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" s="2" customFormat="1" spans="1:4">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5">
-        <v>15</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5">
-        <v>16</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="2:4">
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5">
-        <v>17</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="3:4">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" s="2" customFormat="1" spans="1:4">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5">
-        <v>18</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" s="2" customFormat="1" spans="1:4">
       <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5">
-        <v>19</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" s="2" customFormat="1" spans="1:4">
       <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="5">
-        <v>20</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" s="2" customFormat="1" spans="1:4">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="5">
-        <v>21</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" s="1" customFormat="1" spans="2:4">
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5">
-        <v>22</v>
-      </c>
-      <c r="D27" s="5">
-        <v>1</v>
-      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="3:4">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" s="2" customFormat="1" spans="1:4">
       <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="5">
-        <v>23</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" s="2" customFormat="1" spans="1:4">
       <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="5">
-        <v>24</v>
-      </c>
-      <c r="D29" s="5">
-        <v>1</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" s="2" customFormat="1" spans="1:4">
       <c r="A30" s="1"/>
-      <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="5">
-        <v>25</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" s="2" customFormat="1" spans="1:4">
       <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="5">
-        <v>26</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" s="1" customFormat="1" spans="2:4">
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="5">
-        <v>27</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" s="1" customFormat="1" spans="3:4">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" s="2" customFormat="1" spans="1:4">
       <c r="A33" s="1"/>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="5">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" s="2" customFormat="1" spans="1:4">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5">
-        <v>29</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" s="2" customFormat="1" spans="1:4">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="5">
-        <v>30</v>
-      </c>
-      <c r="D35" s="5">
-        <v>1</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" s="2" customFormat="1" spans="1:4">
       <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="5">
-        <v>31</v>
-      </c>
-      <c r="D36" s="5">
-        <v>1</v>
-      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sync et up to date 2023-08-16
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartProcessConfig@s.xlsx
+++ b/Unity/Assets/Config/Excel/StartConfig/Benchmark/StartProcessConfig@s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12360"/>
+    <workbookView windowWidth="11295" windowHeight="8985"/>
   </bookViews>
   <sheets>
     <sheet name="StartProcessConfig" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Id</t>
   </si>
@@ -22,7 +22,13 @@
     <t>所属机器</t>
   </si>
   <si>
+    <t>外网端口</t>
+  </si>
+  <si>
     <t>MachineId</t>
+  </si>
+  <si>
+    <t>Port</t>
   </si>
   <si>
     <t>int</t>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -60,34 +66,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -101,14 +79,6 @@
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,6 +123,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -198,7 +183,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,49 +225,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,121 +363,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,21 +416,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -457,6 +448,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,148 +519,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -676,52 +682,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1021,13 +1027,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:D36"/>
+  <dimension ref="A3:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.35" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="21.1238938053097" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.7522123893805" style="2" customWidth="1"/>
@@ -1035,84 +1041,114 @@
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4">
+    <row r="3" spans="3:5">
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="3:4">
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5">
       <c r="C5" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="3:4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="3:5">
       <c r="C6" s="5">
         <v>1</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="3:4">
+      <c r="E6" s="5">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="3:5">
       <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="3:4">
+      <c r="E7" s="5">
+        <v>20002</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="3:5">
       <c r="C8" s="5">
         <v>3</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="3:4">
+      <c r="E8" s="5">
+        <v>20003</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="3:5">
       <c r="C9" s="5">
         <v>4</v>
       </c>
       <c r="D9" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="3:4">
+      <c r="E9" s="5">
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="3:5">
       <c r="C10" s="5">
         <v>5</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="3:4">
+      <c r="E10" s="5">
+        <v>20005</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="3:5">
       <c r="C11" s="5">
         <v>6</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="3:4">
+      <c r="E11" s="5">
+        <v>20006</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="3:5">
       <c r="C12" s="5">
         <v>7</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>20007</v>
       </c>
     </row>
     <row r="13" spans="1:4">

</xml_diff>